<commit_message>
export tora object and subject
</commit_message>
<xml_diff>
--- a/ReformaAgraria/wwwroot/template/Template_Object_Subject_Tora.xlsx
+++ b/ReformaAgraria/wwwroot/template/Template_Object_Subject_Tora.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="123820"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erlan\Documents\Docs\Reforma Agraria\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erlan\Documents\Workspaces\Microvac\ReformaAgraria\ReformaAgraria\wwwroot\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+  <si>
+    <t/>
+  </si>
   <si>
     <t>NO</t>
   </si>
@@ -3454,1417 +3457,6 @@
       </rPr>
       <t>INYA</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>U</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>d</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>in</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>MENIKAH</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>D</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>s.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ba</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>g</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>g</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Tah</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>u</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>n</t>
-    </r>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ha</t>
-    </r>
-  </si>
-  <si>
-    <t>Kakao</t>
-  </si>
-  <si>
-    <t>Lorong</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Tah</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>u</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>n</t>
-    </r>
-  </si>
-  <si>
-    <t>Kelapa</t>
-  </si>
-  <si>
-    <t>Nurdin</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Tah</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>u</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>n</t>
-    </r>
-  </si>
-  <si>
-    <t>Tanda</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Tah</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>u</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>n</t>
-    </r>
-  </si>
-  <si>
-    <t>Tatu</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>,5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ha</t>
-    </r>
-  </si>
-  <si>
-    <t>Andi</t>
-  </si>
-  <si>
-    <t>Ifan</t>
-  </si>
-  <si>
-    <t>gazim</t>
-  </si>
-  <si>
-    <t>sukardin</t>
-  </si>
-  <si>
-    <t>Muhlis</t>
-  </si>
-  <si>
-    <t>Basri</t>
-  </si>
-  <si>
-    <t>Nuryadin</t>
-  </si>
-  <si>
-    <t>Jafar</t>
-  </si>
-  <si>
-    <t>SD</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ha</t>
-    </r>
-  </si>
-  <si>
-    <t>Jamal</t>
-  </si>
-  <si>
-    <t>SMP</t>
-  </si>
-  <si>
-    <t>T'o</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Tah</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>u</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>n</t>
-    </r>
-  </si>
-  <si>
-    <t>Lin</t>
-  </si>
-  <si>
-    <t>Cambang</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>U</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>d</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>in</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>T</t>
-    </r>
-  </si>
-  <si>
-    <t>SMA</t>
-  </si>
-  <si>
-    <t>Harina</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>Ba'dia/asludin</t>
-  </si>
-  <si>
-    <t>Nuriati</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>P</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>lis</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-  </si>
-  <si>
-    <t>Kahudin</t>
-  </si>
-  <si>
-    <t>Nasution</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Tah</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>u</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>n</t>
-    </r>
-  </si>
-  <si>
-    <t>Sahlan</t>
-  </si>
-  <si>
-    <t>menikah</t>
-  </si>
-  <si>
-    <t>Alwi</t>
-  </si>
-  <si>
-    <t>palawija</t>
-  </si>
-  <si>
-    <t>Lani</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Tah</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>u</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>n</t>
-    </r>
-  </si>
-  <si>
-    <t>Arma</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Tah</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>u</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>n</t>
-    </r>
-  </si>
-  <si>
-    <t>Dini</t>
-  </si>
-  <si>
-    <t>Moko</t>
-  </si>
-  <si>
-    <t>Bahri</t>
-  </si>
-  <si>
-    <t>Nasir</t>
-  </si>
-  <si>
-    <t>Darman</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>al</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>wija,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>k</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>akao</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>dan</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>cen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>g</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>k</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>h</t>
-    </r>
-  </si>
-  <si>
-    <t>Hendrik</t>
-  </si>
-  <si>
-    <t>Wahidin</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Tah</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>u</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>n</t>
-    </r>
-  </si>
-  <si>
-    <t>Heriyanto</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Tah</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>u</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>n</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>d</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Sa</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>h</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>id</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Tah</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>u</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>n</t>
-    </r>
-  </si>
-  <si>
-    <t>Imran</t>
-  </si>
-  <si>
-    <t>Lukman</t>
-  </si>
-  <si>
-    <t>Munggulangi</t>
-  </si>
-  <si>
-    <t>Toba</t>
-  </si>
-  <si>
-    <t>Hulu Sungai Ore</t>
   </si>
 </sst>
 </file>
@@ -4877,11 +3469,23 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -4896,21 +3500,8 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -4943,7 +3534,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -4967,69 +3558,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5037,86 +3576,58 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5456,7 +3967,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D3" sqref="D3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5469,113 +3980,113 @@
   <sheetData>
     <row r="1" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="B1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="8"/>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="25"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="25"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="25"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="25"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="25"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="25"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="25"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="25"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="25"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D11" s="4"/>
     </row>
@@ -5585,93 +4096,99 @@
         <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
+      <c r="B13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
     </row>
     <row r="14" spans="1:4" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="25"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="25"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" ht="159.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="25"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="25"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="25"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="5">
         <v>3</v>
       </c>
-      <c r="C18" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="27"/>
+      <c r="C18" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="12"/>
     </row>
     <row r="19" spans="1:4" ht="58.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="25"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="25"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="25"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="25"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -5689,10 +4206,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5713,1488 +4230,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="C1" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="D1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="F1" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>39</v>
       </c>
+      <c r="H1" s="16" t="s">
+        <v>40</v>
+      </c>
       <c r="I1" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="J1" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="J1" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="K1" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="L1" s="14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="10">
-        <v>1</v>
-      </c>
-      <c r="B2" s="13" t="s">
+      <c r="M1" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M2" s="13"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="11">
-        <v>2</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" s="13"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="11">
-        <v>3</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I4" s="19"/>
-      <c r="J4" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M4" s="13"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="10">
-        <v>4</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" s="19"/>
-      <c r="J5" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M5" s="13"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="11">
-        <v>5</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" s="19"/>
-      <c r="J6" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="M6" s="13"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="11">
-        <v>6</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I7" s="19"/>
-      <c r="J7" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M7" s="13"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="10">
-        <v>7</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8" s="19"/>
-      <c r="J8" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K8" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="M8" s="13"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="11">
-        <v>8</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" s="19"/>
-      <c r="J9" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M9" s="13"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="11">
-        <v>9</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L10" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M10" s="13"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="10">
-        <v>10</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="M11" s="13"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="11">
-        <v>11</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I12" s="19"/>
-      <c r="J12" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K12" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L12" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M12" s="13"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="11">
-        <v>12</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I13" s="19"/>
-      <c r="J13" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K13" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L13" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M13" s="13"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="10">
-        <v>13</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" s="19"/>
-      <c r="J14" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K14" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="L14" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M14" s="13"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="11">
-        <v>14</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I15" s="19"/>
-      <c r="J15" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K15" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="L15" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="M15" s="13"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="11">
-        <v>15</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I16" s="19"/>
-      <c r="J16" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K16" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="L16" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="M16" s="13"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="10">
-        <v>16</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I17" s="19"/>
-      <c r="J17" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K17" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="L17" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M17" s="13"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="11">
-        <v>17</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I18" s="19"/>
-      <c r="J18" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K18" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="L18" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M18" s="13"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="11">
-        <v>18</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H19" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I19" s="19"/>
-      <c r="J19" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K19" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="L19" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M19" s="13"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="10">
-        <v>19</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I20" s="19"/>
-      <c r="J20" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K20" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="L20" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M20" s="13"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="11">
-        <v>20</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H21" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I21" s="19"/>
-      <c r="J21" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K21" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="L21" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="M21" s="13"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="11">
-        <v>21</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I22" s="19"/>
-      <c r="J22" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K22" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="L22" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="M22" s="13"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="10">
-        <v>22</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I23" s="19"/>
-      <c r="J23" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K23" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="L23" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="M23" s="13"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="11">
-        <v>23</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H24" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I24" s="19"/>
-      <c r="J24" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K24" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="L24" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="M24" s="13"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="11">
-        <v>24</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H25" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I25" s="19"/>
-      <c r="J25" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K25" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="L25" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="M25" s="13"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="10">
-        <v>25</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H26" s="13">
-        <v>5</v>
-      </c>
-      <c r="I26" s="18"/>
-      <c r="J26" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="K26" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="L26" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M26" s="13"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="11">
-        <v>26</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H27" s="13">
-        <v>3</v>
-      </c>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="K27" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L27" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="M27" s="13"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="11">
-        <v>27</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="H28" s="13">
-        <v>6</v>
-      </c>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="K28" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L28" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M28" s="13"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="10">
-        <v>28</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H29" s="13">
-        <v>4</v>
-      </c>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="K29" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L29" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="M29" s="13"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="11">
-        <v>29</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H30" s="13">
-        <v>7</v>
-      </c>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="K30" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L30" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M30" s="13"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="11">
-        <v>30</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H31" s="13">
-        <v>5</v>
-      </c>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="K31" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L31" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M31" s="13"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A32" s="10">
-        <v>31</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F32" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H32" s="13">
-        <v>3</v>
-      </c>
-      <c r="I32" s="13"/>
-      <c r="J32" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="K32" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L32" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M32" s="20"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A33" s="11">
-        <v>32</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H33" s="13">
-        <v>2</v>
-      </c>
-      <c r="I33" s="15"/>
-      <c r="J33" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="K33" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="L33" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M33" s="21"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="11">
-        <v>33</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F34" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H34" s="13">
-        <v>3</v>
-      </c>
-      <c r="I34" s="15"/>
-      <c r="J34" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="K34" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="L34" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="M34" s="19"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A35" s="10">
-        <v>34</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F35" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H35" s="13">
-        <v>3</v>
-      </c>
-      <c r="I35" s="15"/>
-      <c r="J35" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="K35" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="L35" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="M35" s="19"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A36" s="11">
-        <v>35</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F36" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="G36" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H36" s="13">
-        <v>7</v>
-      </c>
-      <c r="I36" s="15"/>
-      <c r="J36" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="K36" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="L36" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="M36" s="19"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" s="11">
-        <v>36</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="G37" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H37" s="13">
-        <v>3</v>
-      </c>
-      <c r="I37" s="15"/>
-      <c r="J37" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="K37" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="L37" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="M37" s="19"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="10">
-        <v>37</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F38" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H38" s="13">
-        <v>5</v>
-      </c>
-      <c r="I38" s="15"/>
-      <c r="J38" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="K38" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="L38" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="M38" s="19"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A39" s="11">
-        <v>38</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G39" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H39" s="13">
-        <v>2</v>
-      </c>
-      <c r="I39" s="15"/>
-      <c r="J39" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="K39" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="L39" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="M39" s="19"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A40" s="11">
-        <v>39</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F40" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G40" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H40" s="13">
-        <v>5</v>
-      </c>
-      <c r="I40" s="15"/>
-      <c r="J40" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="K40" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="L40" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="M40" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>